<commit_message>
fixes some small issues, new data
</commit_message>
<xml_diff>
--- a/data/coordinates.xlsx
+++ b/data/coordinates.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sanf/Downloads/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{873BB3D9-BC9C-2949-8B35-D0A50F1930DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="2000" yWindow="640" windowWidth="16380" windowHeight="13720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="locations for the map" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="locations for the map" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -22,374 +27,371 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="120">
   <si>
-    <t xml:space="preserve">current location</t>
-  </si>
-  <si>
-    <t xml:space="preserve">coordinates</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Google Maps link</t>
-  </si>
-  <si>
-    <t xml:space="preserve">current_location</t>
-  </si>
-  <si>
-    <t xml:space="preserve">google_maps_link</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Musée du Louvre</t>
-  </si>
-  <si>
-    <t xml:space="preserve">48.8611473,2.33802768704666</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://maps.app.goo.gl/JNrz56k6kE74d9nt7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">École nationale supérieure des Beaux-Arts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">48.85713185,2.333843977034844</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://maps.app.goo.gl/kPFmPcJMMEkSMxTe6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Musée des Beaux-Arts de Bordeaux</t>
-  </si>
-  <si>
-    <t xml:space="preserve">44.837340600000005,-0.5806817120198913</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://maps.app.goo.gl/M1T4YHvxMthT1muz5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grand Trianon, Versailles</t>
-  </si>
-  <si>
-    <t xml:space="preserve">48.81495355,2.1050854915515513</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://maps.app.goo.gl/E1YKfFQBt67xBvBs5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Château de Versailles</t>
-  </si>
-  <si>
-    <t xml:space="preserve">48.804425249999994,2.120285270992599</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://maps.app.goo.gl/9WsfPcUsXPJ3TFtSA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Musée des Beaux-Arts de Carcassonne</t>
-  </si>
-  <si>
-    <t xml:space="preserve">43.2124778,2.3553731</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://maps.app.goo.gl/rDXBueTqNW97zNgb8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Musée Calvet, Avignon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">43.9469675,4.8036302</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://maps.app.goo.gl/8w8LgtWQ9xgPiFWz5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Musée des Beaux-Arts d'Arras</t>
-  </si>
-  <si>
-    <t xml:space="preserve">50.292028,2.7736831</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://maps.app.goo.gl/LHXqZSGQWyyJ3Ec58</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Musée des Beaux-Arts de Tours</t>
-  </si>
-  <si>
-    <t xml:space="preserve">47.39526145000001,0.6950591874529539</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://maps.app.goo.gl/meSF1nTzbG22aqji6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Musée de Picardie, Amiens</t>
-  </si>
-  <si>
-    <t xml:space="preserve">49.890586,2.2952183665769486</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://maps.app.goo.gl/PgUB8BgsNy3yanPx7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Musée des Beaux-Arts de Valenciennes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">50.3575723,3.5306353</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://maps.app.goo.gl/qizzCML5CDE6KAaLA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Musée Fabre, Montpellier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">43.6117542,3.8801274326001858</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://maps.app.goo.gl/PNsJovTfXhwdfZ4m7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Musée des Beaux-Arts de Nancy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">48.69357817216553, 6.182368085032326</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://maps.app.goo.gl/HQPG2EXD1fcoBdXG8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Musée de Brou, Bourg-en-Bresse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">46.197474,5.236714886363296</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://maps.app.goo.gl/K7WeqRmZw8ip6KNv6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Musée des Beaux-Arts de Rouen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">49.44473675,1.0945818804156213</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://maps.app.goo.gl/2zG4d8e26EbSpD5k8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mobilier national, Paris</t>
-  </si>
-  <si>
-    <t xml:space="preserve">48.83390555,2.350982932919642</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://maps.app.goo.gl/UiCfEKvr8PkoHx1C8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wallace Collection, London</t>
+    <t>current location</t>
+  </si>
+  <si>
+    <t>coordinates</t>
+  </si>
+  <si>
+    <t>Google Maps link</t>
+  </si>
+  <si>
+    <t>current_location</t>
+  </si>
+  <si>
+    <t>google_maps_link</t>
+  </si>
+  <si>
+    <t>Musée du Louvre</t>
+  </si>
+  <si>
+    <t>48.8611473,2.33802768704666</t>
+  </si>
+  <si>
+    <t>https://maps.app.goo.gl/JNrz56k6kE74d9nt7</t>
+  </si>
+  <si>
+    <t>École nationale supérieure des Beaux-Arts</t>
+  </si>
+  <si>
+    <t>48.85713185,2.333843977034844</t>
+  </si>
+  <si>
+    <t>https://maps.app.goo.gl/kPFmPcJMMEkSMxTe6</t>
+  </si>
+  <si>
+    <t>Musée des Beaux-Arts de Bordeaux</t>
+  </si>
+  <si>
+    <t>44.837340600000005,-0.5806817120198913</t>
+  </si>
+  <si>
+    <t>https://maps.app.goo.gl/M1T4YHvxMthT1muz5</t>
+  </si>
+  <si>
+    <t>Grand Trianon, Versailles</t>
+  </si>
+  <si>
+    <t>48.81495355,2.1050854915515513</t>
+  </si>
+  <si>
+    <t>https://maps.app.goo.gl/E1YKfFQBt67xBvBs5</t>
+  </si>
+  <si>
+    <t>Château de Versailles</t>
+  </si>
+  <si>
+    <t>48.804425249999994,2.120285270992599</t>
+  </si>
+  <si>
+    <t>https://maps.app.goo.gl/9WsfPcUsXPJ3TFtSA</t>
+  </si>
+  <si>
+    <t>Musée des Beaux-Arts de Carcassonne</t>
+  </si>
+  <si>
+    <t>43.2124778,2.3553731</t>
+  </si>
+  <si>
+    <t>https://maps.app.goo.gl/rDXBueTqNW97zNgb8</t>
+  </si>
+  <si>
+    <t>Musée Calvet, Avignon</t>
+  </si>
+  <si>
+    <t>43.9469675,4.8036302</t>
+  </si>
+  <si>
+    <t>https://maps.app.goo.gl/8w8LgtWQ9xgPiFWz5</t>
+  </si>
+  <si>
+    <t>Musée des Beaux-Arts d'Arras</t>
+  </si>
+  <si>
+    <t>50.292028,2.7736831</t>
+  </si>
+  <si>
+    <t>https://maps.app.goo.gl/LHXqZSGQWyyJ3Ec58</t>
+  </si>
+  <si>
+    <t>Musée des Beaux-Arts de Tours</t>
+  </si>
+  <si>
+    <t>47.39526145000001,0.6950591874529539</t>
+  </si>
+  <si>
+    <t>https://maps.app.goo.gl/meSF1nTzbG22aqji6</t>
+  </si>
+  <si>
+    <t>Musée de Picardie, Amiens</t>
+  </si>
+  <si>
+    <t>49.890586,2.2952183665769486</t>
+  </si>
+  <si>
+    <t>https://maps.app.goo.gl/PgUB8BgsNy3yanPx7</t>
+  </si>
+  <si>
+    <t>Musée des Beaux-Arts de Valenciennes</t>
+  </si>
+  <si>
+    <t>50.3575723,3.5306353</t>
+  </si>
+  <si>
+    <t>https://maps.app.goo.gl/qizzCML5CDE6KAaLA</t>
+  </si>
+  <si>
+    <t>Musée Fabre, Montpellier</t>
+  </si>
+  <si>
+    <t>43.6117542,3.8801274326001858</t>
+  </si>
+  <si>
+    <t>https://maps.app.goo.gl/PNsJovTfXhwdfZ4m7</t>
+  </si>
+  <si>
+    <t>Musée des Beaux-Arts de Nancy</t>
+  </si>
+  <si>
+    <t>48.69357817216553, 6.182368085032326</t>
+  </si>
+  <si>
+    <t>https://maps.app.goo.gl/HQPG2EXD1fcoBdXG8</t>
+  </si>
+  <si>
+    <t>Musée de Brou, Bourg-en-Bresse</t>
+  </si>
+  <si>
+    <t>46.197474,5.236714886363296</t>
+  </si>
+  <si>
+    <t>https://maps.app.goo.gl/K7WeqRmZw8ip6KNv6</t>
+  </si>
+  <si>
+    <t>Musée des Beaux-Arts de Rouen</t>
+  </si>
+  <si>
+    <t>49.44473675,1.0945818804156213</t>
+  </si>
+  <si>
+    <t>https://maps.app.goo.gl/2zG4d8e26EbSpD5k8</t>
+  </si>
+  <si>
+    <t>Mobilier national, Paris</t>
+  </si>
+  <si>
+    <t>48.83390555,2.350982932919642</t>
+  </si>
+  <si>
+    <t>https://maps.app.goo.gl/UiCfEKvr8PkoHx1C8</t>
+  </si>
+  <si>
+    <t>Wallace Collection, London</t>
   </si>
   <si>
     <t xml:space="preserve">	51.5175189,-0.15306486208384112</t>
   </si>
   <si>
-    <t xml:space="preserve">https://maps.app.goo.gl/pRmFNrx9pXygJLcE7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Musée Saint-Loup, Troyes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">48.3007334,4.080420707848399</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://maps.app.goo.gl/wTvKF4MypWLRi7Cf8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Musée de la Faïence et des Beaux-arts, Nevers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">46.9861002,3.1545879</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://maps.app.goo.gl/7dy5E4dCiBVLDncz8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Église Saint-Nicolas-du-Chardonnet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">48.84914485,2.350324638719119</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://maps.app.goo.gl/Z54c2gBPSYKcdZqW8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chapelle Saint Paul, Paroisse militaire Saint Charles de Foucauld, Camp de Coëtquidan, Guer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">47.905907147054776, -2.116555206317674</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://maps.app.goo.gl/kYJ1e8PreK4tDUEq5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Église Notre-Dame de Versailles</t>
-  </si>
-  <si>
-    <t xml:space="preserve">48.80796005,2.1290219672161563</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://maps.app.goo.gl/iF77QzuxNpsRXdjc7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Château de Fontainebleau</t>
-  </si>
-  <si>
-    <t xml:space="preserve">48.402116649999996,2.6998510246573746</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://maps.app.goo.gl/8NoBxmzxx6tyHVsb9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Louvre-Lens</t>
-  </si>
-  <si>
-    <t xml:space="preserve">50.430517,2.8062997279999995</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://maps.app.goo.gl/E6cASvP9i6iaHsMr6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">National Gallery of Art, Washington</t>
-  </si>
-  <si>
-    <t xml:space="preserve">38.89131155,-77.01990447478894</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://maps.app.goo.gl/fReM4TzM2qUbYphw6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Château de Fontaine-Henry, Thaon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">49.2744586,-0.44998271421308433</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://maps.app.goo.gl/a6cxvRPEiocZqYzh7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Musée des Beaux Arts de Caen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">49.1862879,-0.3615817</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://maps.app.goo.gl/A6ALeKAT17xTj3fNA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Musée des beaux-arts et d'archéologie Joseph Déchelette, Roanne</t>
-  </si>
-  <si>
-    <t xml:space="preserve">46.034981200000004,4.069250588772453</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://maps.app.goo.gl/tT2hxDkFuTr8yD3b9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Musée des Beaux-Arts de Rennes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">48.1096227,-1.6749412386363636</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://maps.app.goo.gl/P6WK7eRF7cDTLEhs7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Musée de Grenoble</t>
+    <t>https://maps.app.goo.gl/pRmFNrx9pXygJLcE7</t>
+  </si>
+  <si>
+    <t>Musée Saint-Loup, Troyes</t>
+  </si>
+  <si>
+    <t>48.3007334,4.080420707848399</t>
+  </si>
+  <si>
+    <t>https://maps.app.goo.gl/wTvKF4MypWLRi7Cf8</t>
+  </si>
+  <si>
+    <t>Musée de la Faïence et des Beaux-arts, Nevers</t>
+  </si>
+  <si>
+    <t>46.9861002,3.1545879</t>
+  </si>
+  <si>
+    <t>https://maps.app.goo.gl/7dy5E4dCiBVLDncz8</t>
+  </si>
+  <si>
+    <t>Église Saint-Nicolas-du-Chardonnet</t>
+  </si>
+  <si>
+    <t>48.84914485,2.350324638719119</t>
+  </si>
+  <si>
+    <t>https://maps.app.goo.gl/Z54c2gBPSYKcdZqW8</t>
+  </si>
+  <si>
+    <t>Chapelle Saint Paul, Paroisse militaire Saint Charles de Foucauld, Camp de Coëtquidan, Guer</t>
+  </si>
+  <si>
+    <t>47.905907147054776, -2.116555206317674</t>
+  </si>
+  <si>
+    <t>https://maps.app.goo.gl/kYJ1e8PreK4tDUEq5</t>
+  </si>
+  <si>
+    <t>Église Notre-Dame de Versailles</t>
+  </si>
+  <si>
+    <t>48.80796005,2.1290219672161563</t>
+  </si>
+  <si>
+    <t>https://maps.app.goo.gl/iF77QzuxNpsRXdjc7</t>
+  </si>
+  <si>
+    <t>Château de Fontainebleau</t>
+  </si>
+  <si>
+    <t>48.402116649999996,2.6998510246573746</t>
+  </si>
+  <si>
+    <t>https://maps.app.goo.gl/8NoBxmzxx6tyHVsb9</t>
+  </si>
+  <si>
+    <t>Louvre-Lens</t>
+  </si>
+  <si>
+    <t>50.430517,2.8062997279999995</t>
+  </si>
+  <si>
+    <t>https://maps.app.goo.gl/E6cASvP9i6iaHsMr6</t>
+  </si>
+  <si>
+    <t>National Gallery of Art, Washington</t>
+  </si>
+  <si>
+    <t>38.89131155,-77.01990447478894</t>
+  </si>
+  <si>
+    <t>https://maps.app.goo.gl/fReM4TzM2qUbYphw6</t>
+  </si>
+  <si>
+    <t>Château de Fontaine-Henry, Thaon</t>
+  </si>
+  <si>
+    <t>49.2744586,-0.44998271421308433</t>
+  </si>
+  <si>
+    <t>https://maps.app.goo.gl/a6cxvRPEiocZqYzh7</t>
+  </si>
+  <si>
+    <t>Musée des Beaux Arts de Caen</t>
+  </si>
+  <si>
+    <t>49.1862879,-0.3615817</t>
+  </si>
+  <si>
+    <t>https://maps.app.goo.gl/A6ALeKAT17xTj3fNA</t>
+  </si>
+  <si>
+    <t>Musée des beaux-arts et d'archéologie Joseph Déchelette, Roanne</t>
+  </si>
+  <si>
+    <t>46.034981200000004,4.069250588772453</t>
+  </si>
+  <si>
+    <t>https://maps.app.goo.gl/tT2hxDkFuTr8yD3b9</t>
+  </si>
+  <si>
+    <t>Musée des Beaux-Arts de Rennes</t>
+  </si>
+  <si>
+    <t>48.1096227,-1.6749412386363636</t>
+  </si>
+  <si>
+    <t>https://maps.app.goo.gl/P6WK7eRF7cDTLEhs7</t>
+  </si>
+  <si>
+    <t>Musée de Grenoble</t>
   </si>
   <si>
     <t xml:space="preserve">	45.1949735,5.732253035706579</t>
   </si>
   <si>
-    <t xml:space="preserve">https://maps.app.goo.gl/t34r2Xjmh3Rjd1So8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Minneapolis Institute of Art</t>
-  </si>
-  <si>
-    <t xml:space="preserve">44.95859455,-93.27415255541163</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://maps.app.goo.gl/KM5V3xbMxroC7hZQ9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Musée des Beaux-Arts d'Angers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">47.4689171,-0.5545020974552516</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://maps.app.goo.gl/t6sSfqeXVgZBF8MRA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Musée Cognac-Jay, Paris</t>
-  </si>
-  <si>
-    <t xml:space="preserve">48.85812085,2.3616823888956446</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://maps.app.goo.gl/whfa4CB1Q53HHb4k6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Musèe d'Art et d'Histoire, Cholet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">47.05835029234056, -0.8815345501285218</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://maps.app.goo.gl/TtGjfQvrhUknL2HY8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Musée de la Marine, Paris</t>
-  </si>
-  <si>
-    <t xml:space="preserve">48.8618163,2.2873421</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://maps.app.goo.gl/fDrwjRJgkj2Z4RfH6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Musée d’Art et d’Archéologie, Guéret</t>
-  </si>
-  <si>
-    <t xml:space="preserve">46.16600803302257, 1.8717122908705264</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://maps.app.goo.gl/DZaAjQGuEKJXMsrd8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Musée des Beaux-Arts de Lyon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">45.766704700000005,4.833645109701492</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://maps.app.goo.gl/B94Awcv329ZpBbUY6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Private collection (Heirs of the Duchess of Duras)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Private collection</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lost</t>
-  </si>
-  <si>
-    <t xml:space="preserve">unidentified</t>
+    <t>https://maps.app.goo.gl/t34r2Xjmh3Rjd1So8</t>
+  </si>
+  <si>
+    <t>Minneapolis Institute of Art</t>
+  </si>
+  <si>
+    <t>44.95859455,-93.27415255541163</t>
+  </si>
+  <si>
+    <t>https://maps.app.goo.gl/KM5V3xbMxroC7hZQ9</t>
+  </si>
+  <si>
+    <t>Musée des Beaux-Arts d'Angers</t>
+  </si>
+  <si>
+    <t>47.4689171,-0.5545020974552516</t>
+  </si>
+  <si>
+    <t>https://maps.app.goo.gl/t6sSfqeXVgZBF8MRA</t>
+  </si>
+  <si>
+    <t>48.85812085,2.3616823888956446</t>
+  </si>
+  <si>
+    <t>https://maps.app.goo.gl/whfa4CB1Q53HHb4k6</t>
+  </si>
+  <si>
+    <t>Musèe d'Art et d'Histoire, Cholet</t>
+  </si>
+  <si>
+    <t>47.05835029234056, -0.8815345501285218</t>
+  </si>
+  <si>
+    <t>https://maps.app.goo.gl/TtGjfQvrhUknL2HY8</t>
+  </si>
+  <si>
+    <t>Musée de la Marine, Paris</t>
+  </si>
+  <si>
+    <t>48.8618163,2.2873421</t>
+  </si>
+  <si>
+    <t>https://maps.app.goo.gl/fDrwjRJgkj2Z4RfH6</t>
+  </si>
+  <si>
+    <t>Musée d’Art et d’Archéologie, Guéret</t>
+  </si>
+  <si>
+    <t>46.16600803302257, 1.8717122908705264</t>
+  </si>
+  <si>
+    <t>https://maps.app.goo.gl/DZaAjQGuEKJXMsrd8</t>
+  </si>
+  <si>
+    <t>Musée des Beaux-Arts de Lyon</t>
+  </si>
+  <si>
+    <t>45.766704700000005,4.833645109701492</t>
+  </si>
+  <si>
+    <t>https://maps.app.goo.gl/B94Awcv329ZpBbUY6</t>
+  </si>
+  <si>
+    <t>Private collection (Heirs of the Duchess of Duras)</t>
+  </si>
+  <si>
+    <t>Private collection</t>
+  </si>
+  <si>
+    <t>lost</t>
+  </si>
+  <si>
+    <t>unidentified</t>
+  </si>
+  <si>
+    <t>Musée Cognacq-Jay, Paris</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
-  </numFmts>
-  <fonts count="10">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -398,64 +400,37 @@
       <charset val="204"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
-      <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
-      <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
-      <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
-      <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
-      <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
-      <family val="0"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -467,7 +442,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -475,146 +450,93 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+  <cellStyles count="1">
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
     <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="ffffff"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="0e2841"/>
+        <a:srgbClr val="0E2841"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="e8e8e8"/>
+        <a:srgbClr val="E8E8E8"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="156082"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="e97132"/>
+        <a:srgbClr val="E97132"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="196b24"/>
+        <a:srgbClr val="196B24"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="0f9ed5"/>
+        <a:srgbClr val="0F9ED5"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="a02b93"/>
+        <a:srgbClr val="A02B93"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="4ea72e"/>
+        <a:srgbClr val="4EA72E"/>
       </a:accent6>
       <a:hlink>
         <a:srgbClr val="467886"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="96607d"/>
+        <a:srgbClr val="96607D"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Aptos Display" panose="02110004020202020204" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Aptos Narrow" panose="02110004020202020204" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
       </a:minorFont>
@@ -646,7 +568,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
         <a:gradFill>
           <a:gsLst>
@@ -670,7 +592,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -730,33 +652,32 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D517"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.55078125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="42.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="45.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="40.33"/>
+    <col min="1" max="2" width="42.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="45.6640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="40.33203125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -768,7 +689,7 @@
       </c>
       <c r="D1" s="6"/>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
@@ -780,7 +701,7 @@
       </c>
       <c r="D2" s="6"/>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>5</v>
       </c>
@@ -791,7 +712,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>8</v>
       </c>
@@ -802,7 +723,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>11</v>
       </c>
@@ -813,7 +734,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>14</v>
       </c>
@@ -824,7 +745,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>17</v>
       </c>
@@ -835,7 +756,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>20</v>
       </c>
@@ -846,7 +767,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>23</v>
       </c>
@@ -857,7 +778,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>26</v>
       </c>
@@ -868,7 +789,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>29</v>
       </c>
@@ -879,7 +800,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>32</v>
       </c>
@@ -890,7 +811,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
         <v>35</v>
       </c>
@@ -901,7 +822,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
         <v>38</v>
       </c>
@@ -912,7 +833,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
         <v>41</v>
       </c>
@@ -923,7 +844,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
         <v>44</v>
       </c>
@@ -934,7 +855,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>47</v>
       </c>
@@ -945,7 +866,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>50</v>
       </c>
@@ -956,7 +877,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>53</v>
       </c>
@@ -967,7 +888,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
         <v>56</v>
       </c>
@@ -978,7 +899,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
         <v>59</v>
       </c>
@@ -989,7 +910,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
         <v>62</v>
       </c>
@@ -1000,7 +921,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
         <v>65</v>
       </c>
@@ -1011,7 +932,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
         <v>68</v>
       </c>
@@ -1022,7 +943,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
         <v>71</v>
       </c>
@@ -1033,7 +954,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
         <v>74</v>
       </c>
@@ -1044,7 +965,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
         <v>77</v>
       </c>
@@ -1055,7 +976,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
         <v>80</v>
       </c>
@@ -1066,7 +987,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="7" t="s">
         <v>83</v>
       </c>
@@ -1077,7 +998,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A30" s="7" t="s">
         <v>86</v>
       </c>
@@ -1088,7 +1009,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
         <v>89</v>
       </c>
@@ -1099,7 +1020,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
         <v>92</v>
       </c>
@@ -1110,7 +1031,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="7" t="s">
         <v>95</v>
       </c>
@@ -1121,7 +1042,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="7" t="s">
         <v>98</v>
       </c>
@@ -1132,1988 +1053,1983 @@
         <v>100</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="B35" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="B35" s="7" t="s">
+      <c r="C35" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="C35" s="2" t="s">
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="7" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="7" t="s">
+      <c r="B36" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="B36" s="7" t="s">
+      <c r="C36" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="C36" s="2" t="s">
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="7" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="7" t="s">
+      <c r="B37" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="B37" s="7" t="s">
+      <c r="C37" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="C37" s="2" t="s">
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="7" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="7" t="s">
+      <c r="B38" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="B38" s="7" t="s">
+      <c r="C38" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="C38" s="2" t="s">
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="7" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="7" t="s">
+      <c r="B39" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="B39" s="7" t="s">
+      <c r="C39" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="C39" s="2" t="s">
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="7" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="7" t="s">
+      <c r="B40" s="7"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="B40" s="7"/>
-    </row>
-    <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="7" t="s">
+      <c r="B41" s="7"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="B41" s="7"/>
-    </row>
-    <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="7" t="s">
+      <c r="B42" s="7"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="B42" s="7"/>
-    </row>
-    <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="7" t="s">
-        <v>119</v>
-      </c>
       <c r="B43" s="7"/>
     </row>
-    <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
     </row>
-    <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
     </row>
-    <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
     </row>
-    <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
     </row>
-    <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
     </row>
-    <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
     </row>
-    <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
     </row>
-    <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
     </row>
-    <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
     </row>
-    <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
     </row>
-    <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
     </row>
-    <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
     </row>
-    <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
     </row>
-    <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
     </row>
-    <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
     </row>
-    <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
     </row>
-    <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
     </row>
-    <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
     </row>
-    <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
     </row>
-    <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" s="2"/>
       <c r="B63" s="2"/>
     </row>
-    <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
     </row>
-    <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" s="2"/>
       <c r="B65" s="2"/>
     </row>
-    <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" s="2"/>
       <c r="B66" s="2"/>
     </row>
-    <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" s="2"/>
       <c r="B67" s="2"/>
     </row>
-    <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" s="2"/>
       <c r="B68" s="2"/>
     </row>
-    <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" s="2"/>
       <c r="B69" s="2"/>
     </row>
-    <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" s="2"/>
       <c r="B70" s="2"/>
     </row>
-    <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" s="2"/>
       <c r="B71" s="2"/>
     </row>
-    <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" s="2"/>
       <c r="B72" s="2"/>
     </row>
-    <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
     </row>
-    <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" s="2"/>
       <c r="B74" s="2"/>
     </row>
-    <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
     </row>
-    <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" s="2"/>
       <c r="B76" s="2"/>
     </row>
-    <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" s="2"/>
       <c r="B77" s="2"/>
     </row>
-    <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" s="2"/>
       <c r="B78" s="2"/>
     </row>
-    <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" s="2"/>
       <c r="B79" s="2"/>
     </row>
-    <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" s="2"/>
       <c r="B80" s="2"/>
     </row>
-    <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" s="2"/>
       <c r="B81" s="2"/>
     </row>
-    <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" s="2"/>
       <c r="B82" s="2"/>
     </row>
-    <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" s="2"/>
       <c r="B83" s="2"/>
     </row>
-    <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" s="2"/>
       <c r="B84" s="2"/>
     </row>
-    <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" s="2"/>
       <c r="B85" s="2"/>
     </row>
-    <row r="86" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" s="2"/>
       <c r="B86" s="2"/>
     </row>
-    <row r="87" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" s="2"/>
       <c r="B87" s="2"/>
     </row>
-    <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" s="2"/>
       <c r="B88" s="2"/>
     </row>
-    <row r="89" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" s="2"/>
       <c r="B89" s="2"/>
     </row>
-    <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" s="2"/>
       <c r="B90" s="2"/>
     </row>
-    <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" s="2"/>
       <c r="B91" s="2"/>
     </row>
-    <row r="92" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" s="2"/>
       <c r="B92" s="2"/>
     </row>
-    <row r="93" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" s="2"/>
       <c r="B93" s="2"/>
     </row>
-    <row r="94" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" s="2"/>
       <c r="B94" s="2"/>
     </row>
-    <row r="95" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" s="2"/>
       <c r="B95" s="2"/>
     </row>
-    <row r="96" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96" s="2"/>
       <c r="B96" s="2"/>
     </row>
-    <row r="97" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" s="2"/>
       <c r="B97" s="2"/>
     </row>
-    <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" s="2"/>
       <c r="B98" s="2"/>
     </row>
-    <row r="99" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99" s="2"/>
       <c r="B99" s="2"/>
     </row>
-    <row r="100" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100" s="2"/>
       <c r="B100" s="2"/>
     </row>
-    <row r="101" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101" s="2"/>
       <c r="B101" s="2"/>
     </row>
-    <row r="102" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102" s="2"/>
       <c r="B102" s="2"/>
     </row>
-    <row r="103" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103" s="2"/>
       <c r="B103" s="2"/>
     </row>
-    <row r="104" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104" s="2"/>
       <c r="B104" s="2"/>
     </row>
-    <row r="105" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105" s="2"/>
       <c r="B105" s="2"/>
     </row>
-    <row r="106" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106" s="2"/>
       <c r="B106" s="2"/>
     </row>
-    <row r="107" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107" s="2"/>
       <c r="B107" s="2"/>
     </row>
-    <row r="108" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108" s="2"/>
       <c r="B108" s="2"/>
     </row>
-    <row r="109" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109" s="2"/>
       <c r="B109" s="2"/>
     </row>
-    <row r="110" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A110" s="2"/>
       <c r="B110" s="2"/>
     </row>
-    <row r="111" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A111" s="2"/>
       <c r="B111" s="2"/>
     </row>
-    <row r="112" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A112" s="2"/>
       <c r="B112" s="2"/>
     </row>
-    <row r="113" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A113" s="2"/>
       <c r="B113" s="2"/>
     </row>
-    <row r="114" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A114" s="2"/>
       <c r="B114" s="2"/>
     </row>
-    <row r="115" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A115" s="2"/>
       <c r="B115" s="2"/>
     </row>
-    <row r="116" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A116" s="2"/>
       <c r="B116" s="2"/>
     </row>
-    <row r="117" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A117" s="2"/>
       <c r="B117" s="2"/>
     </row>
-    <row r="118" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A118" s="2"/>
       <c r="B118" s="2"/>
     </row>
-    <row r="119" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A119" s="2"/>
       <c r="B119" s="2"/>
     </row>
-    <row r="120" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A120" s="2"/>
       <c r="B120" s="2"/>
     </row>
-    <row r="121" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A121" s="2"/>
       <c r="B121" s="2"/>
     </row>
-    <row r="122" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A122" s="2"/>
       <c r="B122" s="2"/>
     </row>
-    <row r="123" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A123" s="2"/>
       <c r="B123" s="2"/>
     </row>
-    <row r="124" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A124" s="2"/>
       <c r="B124" s="2"/>
     </row>
-    <row r="125" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A125" s="2"/>
       <c r="B125" s="2"/>
     </row>
-    <row r="126" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A126" s="2"/>
       <c r="B126" s="2"/>
     </row>
-    <row r="127" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A127" s="2"/>
       <c r="B127" s="2"/>
     </row>
-    <row r="128" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A128" s="2"/>
       <c r="B128" s="2"/>
     </row>
-    <row r="129" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A129" s="2"/>
       <c r="B129" s="2"/>
     </row>
-    <row r="130" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A130" s="2"/>
       <c r="B130" s="2"/>
     </row>
-    <row r="131" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A131" s="2"/>
       <c r="B131" s="2"/>
     </row>
-    <row r="132" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A132" s="2"/>
       <c r="B132" s="2"/>
     </row>
-    <row r="133" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A133" s="2"/>
       <c r="B133" s="2"/>
     </row>
-    <row r="134" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A134" s="2"/>
       <c r="B134" s="2"/>
     </row>
-    <row r="135" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A135" s="2"/>
       <c r="B135" s="2"/>
     </row>
-    <row r="136" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A136" s="2"/>
       <c r="B136" s="2"/>
     </row>
-    <row r="137" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A137" s="2"/>
       <c r="B137" s="2"/>
     </row>
-    <row r="138" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A138" s="2"/>
       <c r="B138" s="2"/>
     </row>
-    <row r="139" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A139" s="2"/>
       <c r="B139" s="2"/>
     </row>
-    <row r="140" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A140" s="2"/>
       <c r="B140" s="2"/>
     </row>
-    <row r="141" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A141" s="2"/>
       <c r="B141" s="2"/>
     </row>
-    <row r="142" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A142" s="2"/>
       <c r="B142" s="2"/>
     </row>
-    <row r="143" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A143" s="2"/>
       <c r="B143" s="2"/>
     </row>
-    <row r="144" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A144" s="2"/>
       <c r="B144" s="2"/>
     </row>
-    <row r="145" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A145" s="2"/>
       <c r="B145" s="2"/>
     </row>
-    <row r="146" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A146" s="2"/>
       <c r="B146" s="2"/>
     </row>
-    <row r="147" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A147" s="2"/>
       <c r="B147" s="2"/>
     </row>
-    <row r="148" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A148" s="2"/>
       <c r="B148" s="2"/>
     </row>
-    <row r="149" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A149" s="2"/>
       <c r="B149" s="2"/>
     </row>
-    <row r="150" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A150" s="2"/>
       <c r="B150" s="2"/>
     </row>
-    <row r="151" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A151" s="2"/>
       <c r="B151" s="2"/>
     </row>
-    <row r="152" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A152" s="2"/>
       <c r="B152" s="2"/>
     </row>
-    <row r="153" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A153" s="2"/>
       <c r="B153" s="2"/>
     </row>
-    <row r="154" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A154" s="2"/>
       <c r="B154" s="2"/>
     </row>
-    <row r="155" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A155" s="2"/>
       <c r="B155" s="2"/>
     </row>
-    <row r="156" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A156" s="2"/>
       <c r="B156" s="2"/>
     </row>
-    <row r="157" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A157" s="2"/>
       <c r="B157" s="2"/>
     </row>
-    <row r="158" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A158" s="2"/>
       <c r="B158" s="2"/>
     </row>
-    <row r="159" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A159" s="2"/>
       <c r="B159" s="2"/>
     </row>
-    <row r="160" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A160" s="2"/>
       <c r="B160" s="2"/>
     </row>
-    <row r="161" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A161" s="2"/>
       <c r="B161" s="2"/>
     </row>
-    <row r="162" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A162" s="2"/>
       <c r="B162" s="2"/>
     </row>
-    <row r="163" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A163" s="2"/>
       <c r="B163" s="2"/>
     </row>
-    <row r="164" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A164" s="2"/>
       <c r="B164" s="2"/>
     </row>
-    <row r="165" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A165" s="2"/>
       <c r="B165" s="2"/>
     </row>
-    <row r="166" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A166" s="2"/>
       <c r="B166" s="2"/>
     </row>
-    <row r="167" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A167" s="2"/>
       <c r="B167" s="2"/>
     </row>
-    <row r="168" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A168" s="2"/>
       <c r="B168" s="2"/>
     </row>
-    <row r="169" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A169" s="2"/>
       <c r="B169" s="2"/>
     </row>
-    <row r="170" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A170" s="2"/>
       <c r="B170" s="2"/>
     </row>
-    <row r="171" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A171" s="2"/>
       <c r="B171" s="2"/>
     </row>
-    <row r="172" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A172" s="2"/>
       <c r="B172" s="2"/>
     </row>
-    <row r="173" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A173" s="2"/>
       <c r="B173" s="2"/>
     </row>
-    <row r="174" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A174" s="2"/>
       <c r="B174" s="2"/>
     </row>
-    <row r="175" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A175" s="2"/>
       <c r="B175" s="2"/>
     </row>
-    <row r="176" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A176" s="2"/>
       <c r="B176" s="2"/>
     </row>
-    <row r="177" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A177" s="2"/>
       <c r="B177" s="2"/>
     </row>
-    <row r="178" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A178" s="2"/>
       <c r="B178" s="2"/>
     </row>
-    <row r="179" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A179" s="2"/>
       <c r="B179" s="2"/>
     </row>
-    <row r="180" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A180" s="2"/>
       <c r="B180" s="2"/>
     </row>
-    <row r="181" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A181" s="2"/>
       <c r="B181" s="2"/>
     </row>
-    <row r="182" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A182" s="2"/>
       <c r="B182" s="2"/>
     </row>
-    <row r="183" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A183" s="2"/>
       <c r="B183" s="2"/>
     </row>
-    <row r="184" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A184" s="2"/>
       <c r="B184" s="2"/>
     </row>
-    <row r="185" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A185" s="2"/>
       <c r="B185" s="2"/>
     </row>
-    <row r="186" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A186" s="2"/>
       <c r="B186" s="2"/>
     </row>
-    <row r="187" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A187" s="2"/>
       <c r="B187" s="2"/>
     </row>
-    <row r="188" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A188" s="2"/>
       <c r="B188" s="2"/>
     </row>
-    <row r="189" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A189" s="2"/>
       <c r="B189" s="2"/>
     </row>
-    <row r="190" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A190" s="2"/>
       <c r="B190" s="2"/>
     </row>
-    <row r="191" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A191" s="2"/>
       <c r="B191" s="2"/>
     </row>
-    <row r="192" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A192" s="2"/>
       <c r="B192" s="2"/>
     </row>
-    <row r="193" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A193" s="2"/>
       <c r="B193" s="2"/>
     </row>
-    <row r="194" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A194" s="2"/>
       <c r="B194" s="2"/>
     </row>
-    <row r="195" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A195" s="2"/>
       <c r="B195" s="2"/>
     </row>
-    <row r="196" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A196" s="2"/>
       <c r="B196" s="2"/>
     </row>
-    <row r="197" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A197" s="2"/>
       <c r="B197" s="2"/>
     </row>
-    <row r="198" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A198" s="2"/>
       <c r="B198" s="2"/>
     </row>
-    <row r="199" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A199" s="2"/>
       <c r="B199" s="2"/>
     </row>
-    <row r="200" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A200" s="2"/>
       <c r="B200" s="2"/>
     </row>
-    <row r="201" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="201" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A201" s="2"/>
       <c r="B201" s="2"/>
     </row>
-    <row r="202" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="202" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A202" s="2"/>
       <c r="B202" s="2"/>
     </row>
-    <row r="203" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A203" s="2"/>
       <c r="B203" s="2"/>
     </row>
-    <row r="204" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="204" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A204" s="2"/>
       <c r="B204" s="2"/>
     </row>
-    <row r="205" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="205" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A205" s="2"/>
       <c r="B205" s="2"/>
     </row>
-    <row r="206" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A206" s="2"/>
       <c r="B206" s="2"/>
     </row>
-    <row r="207" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="207" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A207" s="2"/>
       <c r="B207" s="2"/>
     </row>
-    <row r="208" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="208" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A208" s="2"/>
       <c r="B208" s="2"/>
     </row>
-    <row r="209" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="209" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A209" s="2"/>
       <c r="B209" s="2"/>
     </row>
-    <row r="210" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="210" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A210" s="2"/>
       <c r="B210" s="2"/>
     </row>
-    <row r="211" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="211" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A211" s="2"/>
       <c r="B211" s="2"/>
     </row>
-    <row r="212" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="212" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A212" s="2"/>
       <c r="B212" s="2"/>
     </row>
-    <row r="213" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="213" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A213" s="2"/>
       <c r="B213" s="2"/>
     </row>
-    <row r="214" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="214" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A214" s="2"/>
       <c r="B214" s="2"/>
     </row>
-    <row r="215" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="215" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A215" s="2"/>
       <c r="B215" s="2"/>
     </row>
-    <row r="216" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="216" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A216" s="2"/>
       <c r="B216" s="2"/>
     </row>
-    <row r="217" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="217" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A217" s="2"/>
       <c r="B217" s="2"/>
     </row>
-    <row r="218" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="218" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A218" s="2"/>
       <c r="B218" s="2"/>
     </row>
-    <row r="219" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="219" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A219" s="2"/>
       <c r="B219" s="2"/>
     </row>
-    <row r="220" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="220" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A220" s="2"/>
       <c r="B220" s="2"/>
     </row>
-    <row r="221" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="221" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A221" s="2"/>
       <c r="B221" s="2"/>
     </row>
-    <row r="222" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="222" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A222" s="2"/>
       <c r="B222" s="2"/>
     </row>
-    <row r="223" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="223" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A223" s="2"/>
       <c r="B223" s="2"/>
     </row>
-    <row r="224" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="224" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A224" s="2"/>
       <c r="B224" s="2"/>
     </row>
-    <row r="225" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="225" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A225" s="2"/>
       <c r="B225" s="2"/>
     </row>
-    <row r="226" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="226" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A226" s="2"/>
       <c r="B226" s="2"/>
     </row>
-    <row r="227" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="227" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A227" s="2"/>
       <c r="B227" s="2"/>
     </row>
-    <row r="228" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="228" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A228" s="2"/>
       <c r="B228" s="2"/>
     </row>
-    <row r="229" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="229" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A229" s="2"/>
       <c r="B229" s="2"/>
     </row>
-    <row r="230" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="230" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A230" s="2"/>
       <c r="B230" s="2"/>
     </row>
-    <row r="231" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="231" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A231" s="2"/>
       <c r="B231" s="2"/>
     </row>
-    <row r="232" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="232" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A232" s="2"/>
       <c r="B232" s="2"/>
     </row>
-    <row r="233" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="233" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A233" s="2"/>
       <c r="B233" s="2"/>
     </row>
-    <row r="234" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="234" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A234" s="2"/>
       <c r="B234" s="2"/>
     </row>
-    <row r="235" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="235" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A235" s="2"/>
       <c r="B235" s="2"/>
     </row>
-    <row r="236" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="236" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A236" s="2"/>
       <c r="B236" s="2"/>
     </row>
-    <row r="237" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="237" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A237" s="2"/>
       <c r="B237" s="2"/>
     </row>
-    <row r="238" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="238" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A238" s="2"/>
       <c r="B238" s="2"/>
     </row>
-    <row r="239" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="239" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A239" s="2"/>
       <c r="B239" s="2"/>
     </row>
-    <row r="240" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="240" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A240" s="2"/>
       <c r="B240" s="2"/>
     </row>
-    <row r="241" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="241" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A241" s="2"/>
       <c r="B241" s="2"/>
     </row>
-    <row r="242" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="242" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A242" s="2"/>
       <c r="B242" s="2"/>
     </row>
-    <row r="243" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="243" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A243" s="2"/>
       <c r="B243" s="2"/>
     </row>
-    <row r="244" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="244" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A244" s="2"/>
       <c r="B244" s="2"/>
     </row>
-    <row r="245" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="245" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A245" s="2"/>
       <c r="B245" s="2"/>
     </row>
-    <row r="246" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="246" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A246" s="2"/>
       <c r="B246" s="2"/>
     </row>
-    <row r="247" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="247" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A247" s="2"/>
       <c r="B247" s="2"/>
     </row>
-    <row r="248" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="248" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A248" s="2"/>
       <c r="B248" s="2"/>
     </row>
-    <row r="249" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="249" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A249" s="2"/>
       <c r="B249" s="2"/>
     </row>
-    <row r="250" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="250" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A250" s="2"/>
       <c r="B250" s="2"/>
     </row>
-    <row r="251" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="251" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A251" s="2"/>
       <c r="B251" s="2"/>
     </row>
-    <row r="252" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="252" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A252" s="2"/>
       <c r="B252" s="2"/>
     </row>
-    <row r="253" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="253" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A253" s="2"/>
       <c r="B253" s="2"/>
     </row>
-    <row r="254" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="254" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A254" s="2"/>
       <c r="B254" s="2"/>
     </row>
-    <row r="255" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="255" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A255" s="2"/>
       <c r="B255" s="2"/>
     </row>
-    <row r="256" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="256" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A256" s="2"/>
       <c r="B256" s="2"/>
     </row>
-    <row r="257" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="257" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A257" s="2"/>
       <c r="B257" s="2"/>
     </row>
-    <row r="258" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="258" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A258" s="2"/>
       <c r="B258" s="2"/>
     </row>
-    <row r="259" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="259" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A259" s="2"/>
       <c r="B259" s="2"/>
     </row>
-    <row r="260" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="260" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A260" s="2"/>
       <c r="B260" s="2"/>
     </row>
-    <row r="261" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="261" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A261" s="2"/>
       <c r="B261" s="2"/>
     </row>
-    <row r="262" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="262" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A262" s="2"/>
       <c r="B262" s="2"/>
     </row>
-    <row r="263" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="263" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A263" s="2"/>
       <c r="B263" s="2"/>
     </row>
-    <row r="264" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="264" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A264" s="2"/>
       <c r="B264" s="2"/>
     </row>
-    <row r="265" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="265" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A265" s="2"/>
       <c r="B265" s="2"/>
     </row>
-    <row r="266" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="266" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A266" s="2"/>
       <c r="B266" s="2"/>
     </row>
-    <row r="267" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="267" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A267" s="2"/>
       <c r="B267" s="2"/>
     </row>
-    <row r="268" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="268" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A268" s="2"/>
       <c r="B268" s="2"/>
     </row>
-    <row r="269" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="269" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A269" s="2"/>
       <c r="B269" s="2"/>
     </row>
-    <row r="270" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="270" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A270" s="2"/>
       <c r="B270" s="2"/>
     </row>
-    <row r="271" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="271" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A271" s="2"/>
       <c r="B271" s="2"/>
     </row>
-    <row r="272" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="272" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A272" s="2"/>
       <c r="B272" s="2"/>
     </row>
-    <row r="273" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="273" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A273" s="2"/>
       <c r="B273" s="2"/>
     </row>
-    <row r="274" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="274" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A274" s="2"/>
       <c r="B274" s="2"/>
     </row>
-    <row r="275" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="275" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A275" s="2"/>
       <c r="B275" s="2"/>
     </row>
-    <row r="276" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="276" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A276" s="2"/>
       <c r="B276" s="2"/>
     </row>
-    <row r="277" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="277" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A277" s="2"/>
       <c r="B277" s="2"/>
     </row>
-    <row r="278" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="278" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A278" s="2"/>
       <c r="B278" s="2"/>
     </row>
-    <row r="279" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="279" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A279" s="2"/>
       <c r="B279" s="2"/>
     </row>
-    <row r="280" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="280" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A280" s="2"/>
       <c r="B280" s="2"/>
     </row>
-    <row r="281" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="281" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A281" s="2"/>
       <c r="B281" s="2"/>
     </row>
-    <row r="282" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="282" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A282" s="2"/>
       <c r="B282" s="2"/>
     </row>
-    <row r="283" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="283" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A283" s="2"/>
       <c r="B283" s="2"/>
     </row>
-    <row r="284" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="284" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A284" s="2"/>
       <c r="B284" s="2"/>
     </row>
-    <row r="285" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="285" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A285" s="2"/>
       <c r="B285" s="2"/>
     </row>
-    <row r="286" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="286" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A286" s="2"/>
       <c r="B286" s="2"/>
     </row>
-    <row r="287" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="287" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A287" s="2"/>
       <c r="B287" s="2"/>
     </row>
-    <row r="288" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="288" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A288" s="2"/>
       <c r="B288" s="2"/>
     </row>
-    <row r="289" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="289" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A289" s="2"/>
       <c r="B289" s="2"/>
     </row>
-    <row r="290" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="290" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A290" s="2"/>
       <c r="B290" s="2"/>
     </row>
-    <row r="291" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="291" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A291" s="2"/>
       <c r="B291" s="2"/>
     </row>
-    <row r="292" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="292" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A292" s="2"/>
       <c r="B292" s="2"/>
     </row>
-    <row r="293" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="293" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A293" s="2"/>
       <c r="B293" s="2"/>
     </row>
-    <row r="294" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="294" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A294" s="2"/>
       <c r="B294" s="2"/>
     </row>
-    <row r="295" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="295" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A295" s="2"/>
       <c r="B295" s="2"/>
     </row>
-    <row r="296" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="296" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A296" s="2"/>
       <c r="B296" s="2"/>
     </row>
-    <row r="297" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="297" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A297" s="2"/>
       <c r="B297" s="2"/>
     </row>
-    <row r="298" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="298" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A298" s="2"/>
       <c r="B298" s="2"/>
     </row>
-    <row r="299" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="299" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A299" s="2"/>
       <c r="B299" s="2"/>
     </row>
-    <row r="300" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="300" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A300" s="2"/>
       <c r="B300" s="2"/>
     </row>
-    <row r="301" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="301" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A301" s="2"/>
       <c r="B301" s="2"/>
     </row>
-    <row r="302" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="302" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A302" s="2"/>
       <c r="B302" s="2"/>
     </row>
-    <row r="303" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="303" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A303" s="2"/>
       <c r="B303" s="2"/>
     </row>
-    <row r="304" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="304" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A304" s="2"/>
       <c r="B304" s="2"/>
     </row>
-    <row r="305" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="305" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A305" s="2"/>
       <c r="B305" s="2"/>
     </row>
-    <row r="306" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="306" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A306" s="2"/>
       <c r="B306" s="2"/>
     </row>
-    <row r="307" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="307" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A307" s="2"/>
       <c r="B307" s="2"/>
     </row>
-    <row r="308" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="308" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A308" s="2"/>
       <c r="B308" s="2"/>
     </row>
-    <row r="309" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="309" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A309" s="2"/>
       <c r="B309" s="2"/>
     </row>
-    <row r="310" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="310" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A310" s="2"/>
       <c r="B310" s="2"/>
     </row>
-    <row r="311" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="311" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A311" s="2"/>
       <c r="B311" s="2"/>
     </row>
-    <row r="312" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="312" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A312" s="2"/>
       <c r="B312" s="2"/>
     </row>
-    <row r="313" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="313" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A313" s="2"/>
       <c r="B313" s="2"/>
     </row>
-    <row r="314" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="314" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A314" s="2"/>
       <c r="B314" s="2"/>
     </row>
-    <row r="315" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="315" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A315" s="2"/>
       <c r="B315" s="2"/>
     </row>
-    <row r="316" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="316" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A316" s="2"/>
       <c r="B316" s="2"/>
     </row>
-    <row r="317" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="317" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A317" s="2"/>
       <c r="B317" s="2"/>
     </row>
-    <row r="318" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="318" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A318" s="2"/>
       <c r="B318" s="2"/>
     </row>
-    <row r="319" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="319" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A319" s="2"/>
       <c r="B319" s="2"/>
     </row>
-    <row r="320" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="320" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A320" s="2"/>
       <c r="B320" s="2"/>
     </row>
-    <row r="321" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="321" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A321" s="2"/>
       <c r="B321" s="2"/>
     </row>
-    <row r="322" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="322" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A322" s="2"/>
       <c r="B322" s="2"/>
     </row>
-    <row r="323" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="323" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A323" s="2"/>
       <c r="B323" s="2"/>
     </row>
-    <row r="324" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="324" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A324" s="2"/>
       <c r="B324" s="2"/>
     </row>
-    <row r="325" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="325" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A325" s="2"/>
       <c r="B325" s="2"/>
     </row>
-    <row r="326" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="326" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A326" s="2"/>
       <c r="B326" s="2"/>
     </row>
-    <row r="327" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="327" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A327" s="2"/>
       <c r="B327" s="2"/>
     </row>
-    <row r="328" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="328" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A328" s="2"/>
       <c r="B328" s="2"/>
     </row>
-    <row r="329" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="329" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A329" s="2"/>
       <c r="B329" s="2"/>
     </row>
-    <row r="330" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="330" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A330" s="2"/>
       <c r="B330" s="2"/>
     </row>
-    <row r="331" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="331" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A331" s="2"/>
       <c r="B331" s="2"/>
     </row>
-    <row r="332" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="332" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A332" s="2"/>
       <c r="B332" s="2"/>
     </row>
-    <row r="333" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="333" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A333" s="2"/>
       <c r="B333" s="2"/>
     </row>
-    <row r="334" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="334" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A334" s="2"/>
       <c r="B334" s="2"/>
     </row>
-    <row r="335" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="335" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A335" s="2"/>
       <c r="B335" s="2"/>
     </row>
-    <row r="336" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="336" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A336" s="2"/>
       <c r="B336" s="2"/>
     </row>
-    <row r="337" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="337" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A337" s="2"/>
       <c r="B337" s="2"/>
     </row>
-    <row r="338" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="338" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A338" s="2"/>
       <c r="B338" s="2"/>
     </row>
-    <row r="339" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="339" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A339" s="2"/>
       <c r="B339" s="2"/>
     </row>
-    <row r="340" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="340" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A340" s="2"/>
       <c r="B340" s="2"/>
     </row>
-    <row r="341" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="341" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A341" s="2"/>
       <c r="B341" s="2"/>
     </row>
-    <row r="342" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="342" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A342" s="2"/>
       <c r="B342" s="2"/>
     </row>
-    <row r="343" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="343" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A343" s="2"/>
       <c r="B343" s="2"/>
     </row>
-    <row r="344" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="344" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A344" s="2"/>
       <c r="B344" s="2"/>
     </row>
-    <row r="345" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="345" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A345" s="2"/>
       <c r="B345" s="2"/>
     </row>
-    <row r="346" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="346" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A346" s="2"/>
       <c r="B346" s="2"/>
     </row>
-    <row r="347" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="347" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A347" s="2"/>
       <c r="B347" s="2"/>
     </row>
-    <row r="348" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="348" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A348" s="2"/>
       <c r="B348" s="2"/>
     </row>
-    <row r="349" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="349" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A349" s="2"/>
       <c r="B349" s="2"/>
     </row>
-    <row r="350" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="350" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A350" s="2"/>
       <c r="B350" s="2"/>
     </row>
-    <row r="351" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="351" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A351" s="2"/>
       <c r="B351" s="2"/>
     </row>
-    <row r="352" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="352" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A352" s="2"/>
       <c r="B352" s="2"/>
     </row>
-    <row r="353" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="353" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A353" s="2"/>
       <c r="B353" s="2"/>
     </row>
-    <row r="354" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="354" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A354" s="2"/>
       <c r="B354" s="2"/>
     </row>
-    <row r="355" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="355" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A355" s="2"/>
       <c r="B355" s="2"/>
     </row>
-    <row r="356" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="356" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A356" s="2"/>
       <c r="B356" s="2"/>
     </row>
-    <row r="357" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="357" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A357" s="2"/>
       <c r="B357" s="2"/>
     </row>
-    <row r="358" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="358" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A358" s="2"/>
       <c r="B358" s="2"/>
     </row>
-    <row r="359" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="359" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A359" s="2"/>
       <c r="B359" s="2"/>
     </row>
-    <row r="360" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="360" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A360" s="2"/>
       <c r="B360" s="2"/>
     </row>
-    <row r="361" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="361" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A361" s="2"/>
       <c r="B361" s="2"/>
     </row>
-    <row r="362" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="362" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A362" s="2"/>
       <c r="B362" s="2"/>
     </row>
-    <row r="363" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="363" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A363" s="2"/>
       <c r="B363" s="2"/>
     </row>
-    <row r="364" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="364" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A364" s="2"/>
       <c r="B364" s="2"/>
     </row>
-    <row r="365" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="365" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A365" s="2"/>
       <c r="B365" s="2"/>
     </row>
-    <row r="366" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="366" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A366" s="2"/>
       <c r="B366" s="2"/>
     </row>
-    <row r="367" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="367" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A367" s="2"/>
       <c r="B367" s="2"/>
     </row>
-    <row r="368" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="368" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A368" s="2"/>
       <c r="B368" s="2"/>
     </row>
-    <row r="369" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="369" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A369" s="2"/>
       <c r="B369" s="2"/>
     </row>
-    <row r="370" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="370" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A370" s="2"/>
       <c r="B370" s="2"/>
     </row>
-    <row r="371" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="371" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A371" s="2"/>
       <c r="B371" s="2"/>
     </row>
-    <row r="372" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="372" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A372" s="2"/>
       <c r="B372" s="2"/>
     </row>
-    <row r="373" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="373" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A373" s="2"/>
       <c r="B373" s="2"/>
     </row>
-    <row r="374" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="374" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A374" s="2"/>
       <c r="B374" s="2"/>
     </row>
-    <row r="375" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="375" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A375" s="2"/>
       <c r="B375" s="2"/>
     </row>
-    <row r="376" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="376" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A376" s="2"/>
       <c r="B376" s="2"/>
     </row>
-    <row r="377" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="377" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A377" s="2"/>
       <c r="B377" s="2"/>
     </row>
-    <row r="378" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="378" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A378" s="2"/>
       <c r="B378" s="2"/>
     </row>
-    <row r="379" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="379" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A379" s="2"/>
       <c r="B379" s="2"/>
     </row>
-    <row r="380" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="380" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A380" s="2"/>
       <c r="B380" s="2"/>
     </row>
-    <row r="381" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="381" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A381" s="2"/>
       <c r="B381" s="2"/>
     </row>
-    <row r="382" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="382" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A382" s="2"/>
       <c r="B382" s="2"/>
     </row>
-    <row r="383" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="383" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A383" s="2"/>
       <c r="B383" s="2"/>
     </row>
-    <row r="384" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="384" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A384" s="2"/>
       <c r="B384" s="2"/>
     </row>
-    <row r="385" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="385" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A385" s="2"/>
       <c r="B385" s="2"/>
     </row>
-    <row r="386" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="386" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A386" s="2"/>
       <c r="B386" s="2"/>
     </row>
-    <row r="387" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="387" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A387" s="2"/>
       <c r="B387" s="2"/>
     </row>
-    <row r="388" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="388" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A388" s="2"/>
       <c r="B388" s="2"/>
     </row>
-    <row r="389" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="389" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A389" s="2"/>
       <c r="B389" s="2"/>
     </row>
-    <row r="390" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="390" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A390" s="2"/>
       <c r="B390" s="2"/>
     </row>
-    <row r="391" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="391" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A391" s="2"/>
       <c r="B391" s="2"/>
     </row>
-    <row r="392" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="392" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A392" s="2"/>
       <c r="B392" s="2"/>
     </row>
-    <row r="393" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="393" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A393" s="2"/>
       <c r="B393" s="2"/>
     </row>
-    <row r="394" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="394" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A394" s="2"/>
       <c r="B394" s="2"/>
     </row>
-    <row r="395" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="395" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A395" s="2"/>
       <c r="B395" s="2"/>
     </row>
-    <row r="396" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="396" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A396" s="2"/>
       <c r="B396" s="2"/>
     </row>
-    <row r="397" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="397" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A397" s="2"/>
       <c r="B397" s="2"/>
     </row>
-    <row r="398" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="398" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A398" s="2"/>
       <c r="B398" s="2"/>
     </row>
-    <row r="399" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="399" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A399" s="2"/>
       <c r="B399" s="2"/>
     </row>
-    <row r="400" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="400" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A400" s="2"/>
       <c r="B400" s="2"/>
     </row>
-    <row r="401" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="401" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A401" s="2"/>
       <c r="B401" s="2"/>
     </row>
-    <row r="402" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="402" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A402" s="2"/>
       <c r="B402" s="2"/>
     </row>
-    <row r="403" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="403" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A403" s="2"/>
       <c r="B403" s="2"/>
     </row>
-    <row r="404" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="404" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A404" s="2"/>
       <c r="B404" s="2"/>
     </row>
-    <row r="405" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="405" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A405" s="2"/>
       <c r="B405" s="2"/>
     </row>
-    <row r="406" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="406" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A406" s="2"/>
       <c r="B406" s="2"/>
     </row>
-    <row r="407" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="407" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A407" s="2"/>
       <c r="B407" s="2"/>
     </row>
-    <row r="408" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="408" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A408" s="2"/>
       <c r="B408" s="2"/>
     </row>
-    <row r="409" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="409" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A409" s="2"/>
       <c r="B409" s="2"/>
     </row>
-    <row r="410" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="410" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A410" s="2"/>
       <c r="B410" s="2"/>
     </row>
-    <row r="411" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="411" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A411" s="2"/>
       <c r="B411" s="2"/>
     </row>
-    <row r="412" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="412" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A412" s="2"/>
       <c r="B412" s="2"/>
     </row>
-    <row r="413" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="413" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A413" s="2"/>
       <c r="B413" s="2"/>
     </row>
-    <row r="414" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="414" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A414" s="2"/>
       <c r="B414" s="2"/>
     </row>
-    <row r="415" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="415" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A415" s="2"/>
       <c r="B415" s="2"/>
     </row>
-    <row r="416" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="416" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A416" s="2"/>
       <c r="B416" s="2"/>
     </row>
-    <row r="417" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="417" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A417" s="2"/>
       <c r="B417" s="2"/>
     </row>
-    <row r="418" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="418" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A418" s="2"/>
       <c r="B418" s="2"/>
     </row>
-    <row r="419" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="419" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A419" s="2"/>
       <c r="B419" s="2"/>
     </row>
-    <row r="420" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="420" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A420" s="2"/>
       <c r="B420" s="2"/>
     </row>
-    <row r="421" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="421" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A421" s="2"/>
       <c r="B421" s="2"/>
     </row>
-    <row r="422" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="422" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A422" s="2"/>
       <c r="B422" s="2"/>
     </row>
-    <row r="423" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="423" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A423" s="2"/>
       <c r="B423" s="2"/>
     </row>
-    <row r="424" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="424" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A424" s="2"/>
       <c r="B424" s="2"/>
     </row>
-    <row r="425" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="425" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A425" s="2"/>
       <c r="B425" s="2"/>
     </row>
-    <row r="426" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="426" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A426" s="2"/>
       <c r="B426" s="2"/>
     </row>
-    <row r="427" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="427" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A427" s="2"/>
       <c r="B427" s="2"/>
     </row>
-    <row r="428" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="428" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A428" s="2"/>
       <c r="B428" s="2"/>
     </row>
-    <row r="429" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="429" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A429" s="2"/>
       <c r="B429" s="2"/>
     </row>
-    <row r="430" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="430" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A430" s="2"/>
       <c r="B430" s="2"/>
     </row>
-    <row r="431" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="431" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A431" s="2"/>
       <c r="B431" s="2"/>
     </row>
-    <row r="432" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="432" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A432" s="2"/>
       <c r="B432" s="2"/>
     </row>
-    <row r="433" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="433" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A433" s="2"/>
       <c r="B433" s="2"/>
     </row>
-    <row r="434" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="434" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A434" s="2"/>
       <c r="B434" s="2"/>
     </row>
-    <row r="435" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="435" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A435" s="2"/>
       <c r="B435" s="2"/>
     </row>
-    <row r="436" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="436" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A436" s="2"/>
       <c r="B436" s="2"/>
     </row>
-    <row r="437" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="437" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A437" s="2"/>
       <c r="B437" s="2"/>
     </row>
-    <row r="438" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="438" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A438" s="2"/>
       <c r="B438" s="2"/>
     </row>
-    <row r="439" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="439" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A439" s="2"/>
       <c r="B439" s="2"/>
     </row>
-    <row r="440" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="440" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A440" s="2"/>
       <c r="B440" s="2"/>
     </row>
-    <row r="441" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="441" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A441" s="2"/>
       <c r="B441" s="2"/>
     </row>
-    <row r="442" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="442" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A442" s="2"/>
       <c r="B442" s="2"/>
     </row>
-    <row r="443" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="443" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A443" s="2"/>
       <c r="B443" s="2"/>
     </row>
-    <row r="444" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="444" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A444" s="2"/>
       <c r="B444" s="2"/>
     </row>
-    <row r="445" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="445" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A445" s="2"/>
       <c r="B445" s="2"/>
     </row>
-    <row r="446" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="446" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A446" s="2"/>
       <c r="B446" s="2"/>
     </row>
-    <row r="447" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="447" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A447" s="2"/>
       <c r="B447" s="2"/>
     </row>
-    <row r="448" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="448" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A448" s="2"/>
       <c r="B448" s="2"/>
     </row>
-    <row r="449" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="449" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A449" s="2"/>
       <c r="B449" s="2"/>
     </row>
-    <row r="450" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="450" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A450" s="2"/>
       <c r="B450" s="2"/>
     </row>
-    <row r="451" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="451" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A451" s="2"/>
       <c r="B451" s="2"/>
     </row>
-    <row r="452" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="452" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A452" s="2"/>
       <c r="B452" s="2"/>
     </row>
-    <row r="453" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="453" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A453" s="2"/>
       <c r="B453" s="2"/>
     </row>
-    <row r="454" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="454" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A454" s="2"/>
       <c r="B454" s="2"/>
     </row>
-    <row r="455" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="455" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A455" s="2"/>
       <c r="B455" s="2"/>
     </row>
-    <row r="456" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="456" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A456" s="2"/>
       <c r="B456" s="2"/>
     </row>
-    <row r="457" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="457" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A457" s="2"/>
       <c r="B457" s="2"/>
     </row>
-    <row r="458" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="458" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A458" s="2"/>
       <c r="B458" s="2"/>
     </row>
-    <row r="459" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="459" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A459" s="2"/>
       <c r="B459" s="2"/>
     </row>
-    <row r="460" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="460" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A460" s="2"/>
       <c r="B460" s="2"/>
     </row>
-    <row r="461" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="461" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A461" s="2"/>
       <c r="B461" s="2"/>
     </row>
-    <row r="462" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="462" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A462" s="2"/>
       <c r="B462" s="2"/>
     </row>
-    <row r="463" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="463" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A463" s="2"/>
       <c r="B463" s="2"/>
     </row>
-    <row r="464" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="464" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A464" s="2"/>
       <c r="B464" s="2"/>
     </row>
-    <row r="465" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="465" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A465" s="2"/>
       <c r="B465" s="2"/>
     </row>
-    <row r="466" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="466" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A466" s="2"/>
       <c r="B466" s="2"/>
     </row>
-    <row r="467" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="467" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A467" s="2"/>
       <c r="B467" s="2"/>
     </row>
-    <row r="468" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="468" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A468" s="2"/>
       <c r="B468" s="2"/>
     </row>
-    <row r="469" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="469" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A469" s="2"/>
       <c r="B469" s="2"/>
     </row>
-    <row r="470" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="470" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A470" s="2"/>
       <c r="B470" s="2"/>
     </row>
-    <row r="471" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="471" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A471" s="2"/>
       <c r="B471" s="2"/>
     </row>
-    <row r="472" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="472" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A472" s="2"/>
       <c r="B472" s="2"/>
     </row>
-    <row r="473" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="473" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A473" s="2"/>
       <c r="B473" s="2"/>
     </row>
-    <row r="474" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="474" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A474" s="2"/>
       <c r="B474" s="2"/>
     </row>
-    <row r="475" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="475" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A475" s="2"/>
       <c r="B475" s="2"/>
     </row>
-    <row r="476" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="476" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A476" s="2"/>
       <c r="B476" s="2"/>
     </row>
-    <row r="477" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="477" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A477" s="2"/>
       <c r="B477" s="2"/>
     </row>
-    <row r="478" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="478" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A478" s="2"/>
       <c r="B478" s="2"/>
     </row>
-    <row r="479" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="479" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A479" s="2"/>
       <c r="B479" s="2"/>
     </row>
-    <row r="480" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="480" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A480" s="2"/>
       <c r="B480" s="2"/>
     </row>
-    <row r="481" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="481" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A481" s="2"/>
       <c r="B481" s="2"/>
     </row>
-    <row r="482" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="482" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A482" s="2"/>
       <c r="B482" s="2"/>
     </row>
-    <row r="483" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="483" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A483" s="2"/>
       <c r="B483" s="2"/>
     </row>
-    <row r="484" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="484" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A484" s="2"/>
       <c r="B484" s="2"/>
     </row>
-    <row r="485" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="485" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A485" s="2"/>
       <c r="B485" s="2"/>
     </row>
-    <row r="486" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="486" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A486" s="2"/>
       <c r="B486" s="2"/>
     </row>
-    <row r="487" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="487" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A487" s="2"/>
       <c r="B487" s="2"/>
     </row>
-    <row r="488" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="488" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A488" s="2"/>
       <c r="B488" s="2"/>
     </row>
-    <row r="489" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="489" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A489" s="2"/>
       <c r="B489" s="2"/>
     </row>
-    <row r="490" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="490" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A490" s="2"/>
       <c r="B490" s="2"/>
     </row>
-    <row r="491" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="491" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A491" s="2"/>
       <c r="B491" s="2"/>
     </row>
-    <row r="492" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="492" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A492" s="2"/>
       <c r="B492" s="2"/>
     </row>
-    <row r="493" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="493" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A493" s="2"/>
       <c r="B493" s="2"/>
     </row>
-    <row r="494" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="494" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A494" s="2"/>
       <c r="B494" s="2"/>
     </row>
-    <row r="495" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="495" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A495" s="2"/>
       <c r="B495" s="2"/>
     </row>
-    <row r="496" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="496" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A496" s="2"/>
       <c r="B496" s="2"/>
     </row>
-    <row r="497" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="497" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A497" s="2"/>
       <c r="B497" s="2"/>
     </row>
-    <row r="498" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="498" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A498" s="2"/>
       <c r="B498" s="2"/>
     </row>
-    <row r="499" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="499" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A499" s="2"/>
       <c r="B499" s="2"/>
     </row>
-    <row r="500" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="500" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A500" s="2"/>
       <c r="B500" s="2"/>
     </row>
-    <row r="501" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="501" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A501" s="2"/>
       <c r="B501" s="2"/>
     </row>
-    <row r="502" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="502" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A502" s="2"/>
       <c r="B502" s="2"/>
     </row>
-    <row r="503" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="503" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A503" s="2"/>
       <c r="B503" s="2"/>
     </row>
-    <row r="504" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="504" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A504" s="2"/>
       <c r="B504" s="2"/>
     </row>
-    <row r="505" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="505" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A505" s="2"/>
       <c r="B505" s="2"/>
     </row>
-    <row r="506" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="506" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A506" s="2"/>
       <c r="B506" s="2"/>
     </row>
-    <row r="507" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="507" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A507" s="2"/>
       <c r="B507" s="2"/>
     </row>
-    <row r="508" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="508" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A508" s="2"/>
       <c r="B508" s="2"/>
     </row>
-    <row r="509" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="509" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A509" s="2"/>
       <c r="B509" s="2"/>
     </row>
-    <row r="510" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="510" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A510" s="2"/>
       <c r="B510" s="2"/>
     </row>
-    <row r="511" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="511" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A511" s="2"/>
       <c r="B511" s="2"/>
     </row>
-    <row r="512" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="512" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A512" s="2"/>
       <c r="B512" s="2"/>
     </row>
-    <row r="513" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="513" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A513" s="2"/>
       <c r="B513" s="2"/>
     </row>
-    <row r="514" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="514" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A514" s="2"/>
       <c r="B514" s="2"/>
     </row>
-    <row r="515" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="515" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A515" s="2"/>
       <c r="B515" s="2"/>
     </row>
-    <row r="516" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="516" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A516" s="2"/>
       <c r="B516" s="2"/>
     </row>
-    <row r="517" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="517" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A517" s="2"/>
       <c r="B517" s="2"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixes issues reported via mail
</commit_message>
<xml_diff>
--- a/data/coordinates.xlsx
+++ b/data/coordinates.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sanf/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sanf/Desktop/Académie Royale Collection/Database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{873BB3D9-BC9C-2949-8B35-D0A50F1930DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{473C0ECF-48F8-A74F-9DDC-02B53C88BD80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2000" yWindow="640" windowWidth="16380" windowHeight="13720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="123">
   <si>
     <t>current location</t>
   </si>
@@ -213,9 +213,6 @@
     <t>https://maps.app.goo.gl/7dy5E4dCiBVLDncz8</t>
   </si>
   <si>
-    <t>Église Saint-Nicolas-du-Chardonnet</t>
-  </si>
-  <si>
     <t>48.84914485,2.350324638719119</t>
   </si>
   <si>
@@ -385,6 +382,18 @@
   </si>
   <si>
     <t>Musée Cognacq-Jay, Paris</t>
+  </si>
+  <si>
+    <t>Petite Écurie, Versailles</t>
+  </si>
+  <si>
+    <t>https://maps.app.goo.gl/K4WFSeB4yK8Dxbvw6</t>
+  </si>
+  <si>
+    <t>48.801905700000006,2.1278436690571345</t>
+  </si>
+  <si>
+    <t>Église Saint-Nicolas-du-Chardonnet, Paris</t>
   </si>
 </sst>
 </file>
@@ -666,8 +675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D517"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -912,232 +921,238 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="B22" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="C22" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B23" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="C23" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B24" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="C24" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B25" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="C25" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B26" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="C26" s="2" t="s">
         <v>75</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B27" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="B27" s="7" t="s">
+      <c r="C27" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="B28" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="B28" s="7" t="s">
+      <c r="C28" s="2" t="s">
         <v>81</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B29" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="B29" s="7" t="s">
+      <c r="C29" s="2" t="s">
         <v>84</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A30" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B30" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="B30" s="7" t="s">
+      <c r="C30" s="2" t="s">
         <v>87</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B31" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="B31" s="7" t="s">
+      <c r="C31" s="2" t="s">
         <v>90</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B32" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="B32" s="7" t="s">
+      <c r="C32" s="2" t="s">
         <v>93</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="B33" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="B33" s="7" t="s">
+      <c r="C33" s="2" t="s">
         <v>96</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B34" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="B34" s="7" t="s">
+      <c r="C34" s="2" t="s">
         <v>99</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B35" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>101</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="B36" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="B36" s="7" t="s">
+      <c r="C36" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B37" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="B37" s="7" t="s">
+      <c r="C37" s="2" t="s">
         <v>107</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="B38" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="B38" s="7" t="s">
+      <c r="C38" s="2" t="s">
         <v>110</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="B39" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="B39" s="7" t="s">
+      <c r="C39" s="2" t="s">
         <v>113</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B40" s="7"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B41" s="7"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B42" s="7"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B43" s="7"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44" s="2"/>
-      <c r="B44" s="2"/>
+      <c r="A44" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45" s="2"/>
       <c r="B45" s="2"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>